<commit_message>
Enhance Salesmen management: add SQL triggers for updating total sales and collections, improve UI components, and fix placeholder text in the salesman form
</commit_message>
<xml_diff>
--- a/Backup/Salesmen.xlsx
+++ b/Backup/Salesmen.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,47 +459,106 @@
           <t>Total_Collections</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>IsDeleted</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ahmed Khan</t>
+          <t>Ali Khan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>03124567890</t>
+          <t>03211234567</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>8000</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bilal Saeed</t>
+          <t>Usman Raza</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>03221234567</t>
+          <t>03009876543</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>4000</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ahmed Sheikh</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>03125552223</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>12</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Tareen</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12324323453</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>